<commit_message>
Moving sleep key to menu and putting mouse key on every keyboard
</commit_message>
<xml_diff>
--- a/docs/Keyboard Designs.xlsx
+++ b/docs/Keyboard Designs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="543" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="332">
   <si>
     <t>A</t>
   </si>
@@ -979,9 +979,6 @@
   </si>
   <si>
     <t>REPEAT LAST</t>
-  </si>
-  <si>
-    <t>MOUSE</t>
   </si>
   <si>
     <t>POSITION:</t>
@@ -1355,7 +1352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1569,12 +1566,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1667,6 +1658,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2499,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AW164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="AC82" sqref="AC82"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="AD73" sqref="AD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2557,10 +2551,10 @@
       <c r="V3" s="38"/>
       <c r="W3" s="5"/>
       <c r="X3" s="5"/>
-      <c r="Z3" s="135"/>
-      <c r="AA3" s="135"/>
-      <c r="AB3" s="135"/>
-      <c r="AC3" s="135"/>
+      <c r="Z3" s="134"/>
+      <c r="AA3" s="134"/>
+      <c r="AB3" s="134"/>
+      <c r="AC3" s="134"/>
       <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
       <c r="AJ3" s="5"/>
@@ -2580,10 +2574,10 @@
     </row>
     <row r="4" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="B4" s="116" t="s">
+      <c r="B4" s="115" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="116"/>
+      <c r="C4" s="115"/>
       <c r="D4" s="38" t="s">
         <v>0</v>
       </c>
@@ -2624,10 +2618,10 @@
         <v>37</v>
       </c>
       <c r="W4" s="52"/>
-      <c r="Z4" s="136"/>
-      <c r="AA4" s="136"/>
-      <c r="AB4" s="136"/>
-      <c r="AC4" s="136"/>
+      <c r="Z4" s="135"/>
+      <c r="AA4" s="135"/>
+      <c r="AB4" s="135"/>
+      <c r="AC4" s="135"/>
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
       <c r="AJ4" s="5"/>
@@ -2709,18 +2703,18 @@
     </row>
     <row r="6" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="103"/>
-      <c r="D6" s="103" t="s">
+      <c r="C6" s="101"/>
+      <c r="D6" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="103"/>
-      <c r="F6" s="103" t="s">
+      <c r="E6" s="101"/>
+      <c r="F6" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="103"/>
+      <c r="G6" s="101"/>
       <c r="H6" s="51" t="s">
         <v>28</v>
       </c>
@@ -2736,11 +2730,11 @@
       </c>
       <c r="O6" s="52"/>
       <c r="P6" s="38" t="s">
-        <v>43</v>
+        <v>327</v>
       </c>
       <c r="Q6" s="38"/>
       <c r="R6" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S6" s="59"/>
       <c r="T6" s="49" t="s">
@@ -2809,22 +2803,22 @@
       </c>
     </row>
     <row r="9" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="118">
+      <c r="B9" s="117">
         <v>1</v>
       </c>
-      <c r="C9" s="118"/>
-      <c r="D9" s="118">
+      <c r="C9" s="117"/>
+      <c r="D9" s="117">
         <v>2</v>
       </c>
-      <c r="E9" s="118"/>
+      <c r="E9" s="117"/>
       <c r="F9" s="38">
         <v>3</v>
       </c>
       <c r="G9" s="38"/>
-      <c r="H9" s="107">
+      <c r="H9" s="106">
         <v>4</v>
       </c>
-      <c r="I9" s="107"/>
+      <c r="I9" s="106"/>
       <c r="J9" s="38">
         <v>5</v>
       </c>
@@ -2875,50 +2869,50 @@
     </row>
     <row r="10" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="B10" s="113" t="s">
+      <c r="B10" s="112" t="s">
         <v>55</v>
       </c>
-      <c r="C10" s="114"/>
-      <c r="D10" s="113" t="s">
+      <c r="C10" s="113"/>
+      <c r="D10" s="112" t="s">
         <v>83</v>
       </c>
-      <c r="E10" s="114"/>
-      <c r="F10" s="109" t="s">
+      <c r="E10" s="113"/>
+      <c r="F10" s="108" t="s">
         <v>79</v>
       </c>
-      <c r="G10" s="109"/>
-      <c r="H10" s="115" t="s">
+      <c r="G10" s="108"/>
+      <c r="H10" s="114" t="s">
         <v>54</v>
       </c>
-      <c r="I10" s="109"/>
-      <c r="J10" s="109" t="s">
+      <c r="I10" s="108"/>
+      <c r="J10" s="108" t="s">
         <v>45</v>
       </c>
-      <c r="K10" s="109"/>
-      <c r="L10" s="109" t="s">
+      <c r="K10" s="108"/>
+      <c r="L10" s="108" t="s">
         <v>78</v>
       </c>
-      <c r="M10" s="109"/>
-      <c r="N10" s="110" t="s">
+      <c r="M10" s="108"/>
+      <c r="N10" s="109" t="s">
         <v>46</v>
       </c>
-      <c r="O10" s="111"/>
-      <c r="P10" s="110" t="s">
+      <c r="O10" s="110"/>
+      <c r="P10" s="109" t="s">
         <v>47</v>
       </c>
-      <c r="Q10" s="111"/>
-      <c r="R10" s="110" t="s">
+      <c r="Q10" s="110"/>
+      <c r="R10" s="109" t="s">
         <v>48</v>
       </c>
-      <c r="S10" s="111"/>
-      <c r="T10" s="110" t="s">
+      <c r="S10" s="110"/>
+      <c r="T10" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="U10" s="111"/>
-      <c r="V10" s="112" t="s">
+      <c r="U10" s="110"/>
+      <c r="V10" s="111" t="s">
         <v>37</v>
       </c>
-      <c r="W10" s="112"/>
+      <c r="W10" s="111"/>
       <c r="Z10" s="3"/>
       <c r="AA10" s="3"/>
       <c r="AH10" s="5"/>
@@ -2956,15 +2950,15 @@
         <v>121</v>
       </c>
       <c r="I11" s="38"/>
-      <c r="J11" s="107" t="s">
+      <c r="J11" s="106" t="s">
         <v>53</v>
       </c>
       <c r="K11" s="38"/>
-      <c r="L11" s="107" t="s">
+      <c r="L11" s="106" t="s">
         <v>84</v>
       </c>
       <c r="M11" s="38"/>
-      <c r="N11" s="107" t="s">
+      <c r="N11" s="106" t="s">
         <v>50</v>
       </c>
       <c r="O11" s="38"/>
@@ -3010,22 +3004,22 @@
     </row>
     <row r="12" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="103" t="s">
+      <c r="B12" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="103"/>
-      <c r="D12" s="103" t="s">
+      <c r="C12" s="101"/>
+      <c r="D12" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E12" s="103"/>
-      <c r="F12" s="103" t="s">
+      <c r="E12" s="101"/>
+      <c r="F12" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G12" s="103"/>
-      <c r="H12" s="106" t="s">
+      <c r="G12" s="101"/>
+      <c r="H12" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="I12" s="106"/>
+      <c r="I12" s="105"/>
       <c r="J12" s="51" t="s">
         <v>26</v>
       </c>
@@ -3036,12 +3030,12 @@
         <v>29</v>
       </c>
       <c r="O12" s="52"/>
-      <c r="P12" s="75" t="s">
+      <c r="P12" s="73" t="s">
         <v>56</v>
       </c>
-      <c r="Q12" s="76"/>
+      <c r="Q12" s="74"/>
       <c r="R12" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S12" s="59"/>
       <c r="T12" s="49" t="s">
@@ -3129,18 +3123,18 @@
         <v>70</v>
       </c>
       <c r="G15" s="47"/>
-      <c r="H15" s="101" t="s">
+      <c r="H15" s="99" t="s">
         <v>81</v>
       </c>
-      <c r="I15" s="102"/>
+      <c r="I15" s="100"/>
       <c r="J15" s="45" t="s">
         <v>62</v>
       </c>
       <c r="K15" s="47"/>
-      <c r="L15" s="101" t="s">
+      <c r="L15" s="99" t="s">
         <v>122</v>
       </c>
-      <c r="M15" s="102"/>
+      <c r="M15" s="100"/>
       <c r="N15" s="45" t="s">
         <v>64</v>
       </c>
@@ -3193,10 +3187,10 @@
         <v>110</v>
       </c>
       <c r="M16" s="38"/>
-      <c r="N16" s="108" t="s">
+      <c r="N16" s="107" t="s">
         <v>71</v>
       </c>
-      <c r="O16" s="108"/>
+      <c r="O16" s="107"/>
       <c r="P16" s="38" t="s">
         <v>72</v>
       </c>
@@ -3209,10 +3203,10 @@
         <v>74</v>
       </c>
       <c r="U16" s="38"/>
-      <c r="V16" s="106" t="s">
+      <c r="V16" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W16" s="106"/>
+      <c r="W16" s="105"/>
       <c r="AA16" s="8"/>
       <c r="AB16" s="8"/>
       <c r="AC16" s="8"/>
@@ -3258,7 +3252,7 @@
       </c>
       <c r="M17" s="38"/>
       <c r="N17" s="38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="O17" s="38"/>
       <c r="P17" s="38" t="s">
@@ -3300,38 +3294,38 @@
     </row>
     <row r="18" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="B18" s="103" t="s">
+      <c r="B18" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="103"/>
-      <c r="D18" s="103" t="s">
+      <c r="C18" s="101"/>
+      <c r="D18" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E18" s="103"/>
-      <c r="F18" s="103" t="s">
+      <c r="E18" s="101"/>
+      <c r="F18" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="103"/>
-      <c r="H18" s="108" t="s">
+      <c r="G18" s="101"/>
+      <c r="H18" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="I18" s="108"/>
+      <c r="I18" s="107"/>
       <c r="J18" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K18" s="53"/>
       <c r="L18" s="53"/>
       <c r="M18" s="53"/>
-      <c r="N18" s="108" t="s">
+      <c r="N18" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="O18" s="108"/>
+      <c r="O18" s="107"/>
       <c r="P18" s="38" t="s">
         <v>82</v>
       </c>
       <c r="Q18" s="38"/>
       <c r="R18" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S18" s="59"/>
       <c r="T18" s="49" t="s">
@@ -3416,18 +3410,18 @@
         <v>140</v>
       </c>
       <c r="G21" s="38"/>
-      <c r="H21" s="119" t="s">
+      <c r="H21" s="118" t="s">
         <v>141</v>
       </c>
-      <c r="I21" s="119"/>
+      <c r="I21" s="118"/>
       <c r="J21" s="38" t="s">
         <v>142</v>
       </c>
       <c r="K21" s="38"/>
-      <c r="L21" s="119" t="s">
+      <c r="L21" s="118" t="s">
         <v>143</v>
       </c>
-      <c r="M21" s="119"/>
+      <c r="M21" s="118"/>
       <c r="N21" s="38" t="s">
         <v>144</v>
       </c>
@@ -3468,18 +3462,18 @@
         <v>150</v>
       </c>
       <c r="G22" s="47"/>
-      <c r="H22" s="101" t="s">
+      <c r="H22" s="99" t="s">
         <v>111</v>
       </c>
-      <c r="I22" s="102"/>
+      <c r="I22" s="100"/>
       <c r="J22" s="45" t="s">
         <v>151</v>
       </c>
       <c r="K22" s="47"/>
-      <c r="L22" s="101" t="s">
+      <c r="L22" s="99" t="s">
         <v>152</v>
       </c>
-      <c r="M22" s="102"/>
+      <c r="M22" s="100"/>
       <c r="N22" s="45" t="s">
         <v>153</v>
       </c>
@@ -3496,10 +3490,10 @@
         <v>156</v>
       </c>
       <c r="U22" s="38"/>
-      <c r="V22" s="106" t="s">
+      <c r="V22" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W22" s="106"/>
+      <c r="W22" s="105"/>
       <c r="AA22" s="8"/>
       <c r="AB22" s="8"/>
       <c r="AC22" s="8"/>
@@ -3525,7 +3519,7 @@
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E23" s="38"/>
       <c r="F23" s="38" t="s">
@@ -3591,38 +3585,38 @@
     </row>
     <row r="24" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
-      <c r="B24" s="103" t="s">
+      <c r="B24" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="103"/>
-      <c r="D24" s="103" t="s">
+      <c r="C24" s="101"/>
+      <c r="D24" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E24" s="103"/>
-      <c r="F24" s="103" t="s">
+      <c r="E24" s="101"/>
+      <c r="F24" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G24" s="103"/>
-      <c r="H24" s="108" t="s">
+      <c r="G24" s="101"/>
+      <c r="H24" s="107" t="s">
         <v>165</v>
       </c>
-      <c r="I24" s="108"/>
+      <c r="I24" s="107"/>
       <c r="J24" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K24" s="53"/>
       <c r="L24" s="53"/>
       <c r="M24" s="53"/>
-      <c r="N24" s="108" t="s">
+      <c r="N24" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="O24" s="108"/>
-      <c r="P24" s="108" t="s">
+      <c r="O24" s="107"/>
+      <c r="P24" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="Q24" s="108"/>
+      <c r="Q24" s="107"/>
       <c r="R24" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S24" s="59"/>
       <c r="T24" s="49" t="s">
@@ -3696,24 +3690,24 @@
     </row>
     <row r="27" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1"/>
-      <c r="B27" s="75" t="s">
-        <v>324</v>
-      </c>
-      <c r="C27" s="118"/>
-      <c r="D27" s="118"/>
-      <c r="E27" s="118"/>
-      <c r="F27" s="118"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="118"/>
-      <c r="I27" s="75" t="s">
+      <c r="B27" s="73" t="s">
+        <v>323</v>
+      </c>
+      <c r="C27" s="117"/>
+      <c r="D27" s="117"/>
+      <c r="E27" s="117"/>
+      <c r="F27" s="117"/>
+      <c r="G27" s="117"/>
+      <c r="H27" s="117"/>
+      <c r="I27" s="73" t="s">
         <v>291</v>
       </c>
-      <c r="J27" s="118"/>
-      <c r="K27" s="118"/>
-      <c r="L27" s="118"/>
-      <c r="M27" s="118"/>
-      <c r="N27" s="118"/>
-      <c r="O27" s="118"/>
+      <c r="J27" s="117"/>
+      <c r="K27" s="117"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="117"/>
+      <c r="N27" s="117"/>
+      <c r="O27" s="117"/>
       <c r="P27" s="62" t="s">
         <v>292</v>
       </c>
@@ -3750,20 +3744,20 @@
     </row>
     <row r="28" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="1"/>
-      <c r="B28" s="118"/>
-      <c r="C28" s="118"/>
-      <c r="D28" s="118"/>
-      <c r="E28" s="118"/>
-      <c r="F28" s="118"/>
-      <c r="G28" s="118"/>
-      <c r="H28" s="118"/>
-      <c r="I28" s="118"/>
-      <c r="J28" s="118"/>
-      <c r="K28" s="118"/>
-      <c r="L28" s="118"/>
-      <c r="M28" s="118"/>
-      <c r="N28" s="118"/>
-      <c r="O28" s="118"/>
+      <c r="B28" s="117"/>
+      <c r="C28" s="117"/>
+      <c r="D28" s="117"/>
+      <c r="E28" s="117"/>
+      <c r="F28" s="117"/>
+      <c r="G28" s="117"/>
+      <c r="H28" s="117"/>
+      <c r="I28" s="117"/>
+      <c r="J28" s="117"/>
+      <c r="K28" s="117"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="117"/>
+      <c r="N28" s="117"/>
+      <c r="O28" s="117"/>
       <c r="P28" s="65"/>
       <c r="Q28" s="66"/>
       <c r="R28" s="66"/>
@@ -3796,26 +3790,26 @@
     </row>
     <row r="29" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1"/>
-      <c r="B29" s="118" t="s">
+      <c r="B29" s="117" t="s">
         <v>295</v>
       </c>
-      <c r="C29" s="118"/>
-      <c r="D29" s="118"/>
-      <c r="E29" s="118"/>
-      <c r="F29" s="118"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="118"/>
-      <c r="I29" s="118" t="s">
+      <c r="C29" s="117"/>
+      <c r="D29" s="117"/>
+      <c r="E29" s="117"/>
+      <c r="F29" s="117"/>
+      <c r="G29" s="117"/>
+      <c r="H29" s="117"/>
+      <c r="I29" s="117" t="s">
+        <v>324</v>
+      </c>
+      <c r="J29" s="117"/>
+      <c r="K29" s="117"/>
+      <c r="L29" s="117"/>
+      <c r="M29" s="117"/>
+      <c r="N29" s="117"/>
+      <c r="O29" s="117"/>
+      <c r="P29" s="62" t="s">
         <v>325</v>
-      </c>
-      <c r="J29" s="118"/>
-      <c r="K29" s="118"/>
-      <c r="L29" s="118"/>
-      <c r="M29" s="118"/>
-      <c r="N29" s="118"/>
-      <c r="O29" s="118"/>
-      <c r="P29" s="62" t="s">
-        <v>326</v>
       </c>
       <c r="Q29" s="63"/>
       <c r="R29" s="63"/>
@@ -3852,20 +3846,20 @@
     </row>
     <row r="30" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="1"/>
-      <c r="B30" s="118"/>
-      <c r="C30" s="118"/>
-      <c r="D30" s="118"/>
-      <c r="E30" s="118"/>
-      <c r="F30" s="118"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="118"/>
-      <c r="I30" s="118"/>
-      <c r="J30" s="118"/>
-      <c r="K30" s="118"/>
-      <c r="L30" s="118"/>
-      <c r="M30" s="118"/>
-      <c r="N30" s="118"/>
-      <c r="O30" s="118"/>
+      <c r="B30" s="117"/>
+      <c r="C30" s="117"/>
+      <c r="D30" s="117"/>
+      <c r="E30" s="117"/>
+      <c r="F30" s="117"/>
+      <c r="G30" s="117"/>
+      <c r="H30" s="117"/>
+      <c r="I30" s="117"/>
+      <c r="J30" s="117"/>
+      <c r="K30" s="117"/>
+      <c r="L30" s="117"/>
+      <c r="M30" s="117"/>
+      <c r="N30" s="117"/>
+      <c r="O30" s="117"/>
       <c r="P30" s="65"/>
       <c r="Q30" s="66"/>
       <c r="R30" s="66"/>
@@ -3953,18 +3947,18 @@
         <v>168</v>
       </c>
       <c r="G33" s="47"/>
-      <c r="H33" s="101" t="s">
+      <c r="H33" s="99" t="s">
         <v>169</v>
       </c>
-      <c r="I33" s="102"/>
+      <c r="I33" s="100"/>
       <c r="J33" s="45" t="s">
         <v>76</v>
       </c>
       <c r="K33" s="47"/>
-      <c r="L33" s="101" t="s">
+      <c r="L33" s="99" t="s">
         <v>170</v>
       </c>
-      <c r="M33" s="102"/>
+      <c r="M33" s="100"/>
       <c r="N33" s="45" t="s">
         <v>171</v>
       </c>
@@ -4017,10 +4011,10 @@
         <v>178</v>
       </c>
       <c r="M34" s="38"/>
-      <c r="N34" s="108" t="s">
+      <c r="N34" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="O34" s="108"/>
+      <c r="O34" s="107"/>
       <c r="P34" s="38" t="s">
         <v>180</v>
       </c>
@@ -4033,10 +4027,10 @@
         <v>182</v>
       </c>
       <c r="U34" s="38"/>
-      <c r="V34" s="106" t="s">
+      <c r="V34" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W34" s="106"/>
+      <c r="W34" s="105"/>
       <c r="AA34" s="8"/>
       <c r="AB34" s="8"/>
       <c r="AC34" s="8"/>
@@ -4089,10 +4083,10 @@
         <v>188</v>
       </c>
       <c r="Q35" s="38"/>
-      <c r="R35" s="117" t="s">
+      <c r="R35" s="116" t="s">
         <v>99</v>
       </c>
-      <c r="S35" s="117"/>
+      <c r="S35" s="116"/>
       <c r="T35" s="56" t="s">
         <v>30</v>
       </c>
@@ -4128,38 +4122,38 @@
     </row>
     <row r="36" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="1"/>
-      <c r="B36" s="103" t="s">
+      <c r="B36" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="103"/>
-      <c r="D36" s="103" t="s">
+      <c r="C36" s="101"/>
+      <c r="D36" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E36" s="103"/>
-      <c r="F36" s="103" t="s">
+      <c r="E36" s="101"/>
+      <c r="F36" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G36" s="103"/>
-      <c r="H36" s="108" t="s">
+      <c r="G36" s="101"/>
+      <c r="H36" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="I36" s="108"/>
+      <c r="I36" s="107"/>
       <c r="J36" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K36" s="53"/>
       <c r="L36" s="53"/>
       <c r="M36" s="53"/>
-      <c r="N36" s="108" t="s">
+      <c r="N36" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="O36" s="108"/>
+      <c r="O36" s="107"/>
       <c r="P36" s="38" t="s">
         <v>191</v>
       </c>
       <c r="Q36" s="45"/>
       <c r="R36" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S36" s="59"/>
       <c r="T36" s="49" t="s">
@@ -4232,18 +4226,18 @@
       </c>
     </row>
     <row r="39" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="119" t="s">
+      <c r="B39" s="118" t="s">
         <v>192</v>
       </c>
-      <c r="C39" s="119"/>
+      <c r="C39" s="118"/>
       <c r="D39" s="38" t="s">
         <v>193</v>
       </c>
       <c r="E39" s="38"/>
-      <c r="F39" s="119" t="s">
+      <c r="F39" s="118" t="s">
         <v>194</v>
       </c>
-      <c r="G39" s="119"/>
+      <c r="G39" s="118"/>
       <c r="H39" s="38" t="s">
         <v>63</v>
       </c>
@@ -4296,18 +4290,18 @@
       <c r="K40" s="47"/>
       <c r="L40" s="38"/>
       <c r="M40" s="38"/>
-      <c r="N40" s="108"/>
-      <c r="O40" s="108"/>
+      <c r="N40" s="107"/>
+      <c r="O40" s="107"/>
       <c r="P40" s="38"/>
       <c r="Q40" s="38"/>
       <c r="R40" s="38"/>
       <c r="S40" s="38"/>
       <c r="T40" s="38"/>
       <c r="U40" s="38"/>
-      <c r="V40" s="106" t="s">
+      <c r="V40" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W40" s="106"/>
+      <c r="W40" s="105"/>
       <c r="AA40" s="8"/>
       <c r="AB40" s="8"/>
       <c r="AC40" s="8"/>
@@ -4385,32 +4379,32 @@
     </row>
     <row r="42" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="1"/>
-      <c r="B42" s="103" t="s">
+      <c r="B42" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="103"/>
-      <c r="D42" s="103" t="s">
+      <c r="C42" s="101"/>
+      <c r="D42" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E42" s="103"/>
-      <c r="F42" s="103" t="s">
+      <c r="E42" s="101"/>
+      <c r="F42" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G42" s="103"/>
-      <c r="H42" s="108"/>
-      <c r="I42" s="108"/>
+      <c r="G42" s="101"/>
+      <c r="H42" s="107"/>
+      <c r="I42" s="107"/>
       <c r="J42" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K42" s="53"/>
       <c r="L42" s="53"/>
       <c r="M42" s="53"/>
-      <c r="N42" s="108"/>
-      <c r="O42" s="108"/>
+      <c r="N42" s="107"/>
+      <c r="O42" s="107"/>
       <c r="P42" s="38"/>
       <c r="Q42" s="38"/>
       <c r="R42" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S42" s="59"/>
       <c r="T42" s="49" t="s">
@@ -4486,18 +4480,18 @@
       </c>
     </row>
     <row r="45" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B45" s="119" t="s">
+      <c r="B45" s="118" t="s">
         <v>202</v>
       </c>
-      <c r="C45" s="119"/>
+      <c r="C45" s="118"/>
       <c r="D45" s="38" t="s">
         <v>203</v>
       </c>
       <c r="E45" s="38"/>
-      <c r="F45" s="119" t="s">
+      <c r="F45" s="118" t="s">
         <v>204</v>
       </c>
-      <c r="G45" s="119"/>
+      <c r="G45" s="118"/>
       <c r="H45" s="38" t="s">
         <v>205</v>
       </c>
@@ -4562,10 +4556,10 @@
         <v>217</v>
       </c>
       <c r="M46" s="38"/>
-      <c r="N46" s="108" t="s">
+      <c r="N46" s="107" t="s">
         <v>218</v>
       </c>
-      <c r="O46" s="108"/>
+      <c r="O46" s="107"/>
       <c r="P46" s="38" t="s">
         <v>219</v>
       </c>
@@ -4578,10 +4572,10 @@
         <v>221</v>
       </c>
       <c r="U46" s="38"/>
-      <c r="V46" s="106" t="s">
+      <c r="V46" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W46" s="106"/>
+      <c r="W46" s="105"/>
       <c r="AA46" s="8"/>
       <c r="AB46" s="8"/>
       <c r="AC46" s="8"/>
@@ -4673,38 +4667,38 @@
     </row>
     <row r="48" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="1"/>
-      <c r="B48" s="103" t="s">
+      <c r="B48" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C48" s="103"/>
-      <c r="D48" s="103" t="s">
+      <c r="C48" s="101"/>
+      <c r="D48" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E48" s="103"/>
-      <c r="F48" s="103" t="s">
+      <c r="E48" s="101"/>
+      <c r="F48" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G48" s="103"/>
-      <c r="H48" s="108" t="s">
+      <c r="G48" s="101"/>
+      <c r="H48" s="107" t="s">
         <v>229</v>
       </c>
-      <c r="I48" s="108"/>
+      <c r="I48" s="107"/>
       <c r="J48" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K48" s="53"/>
       <c r="L48" s="53"/>
       <c r="M48" s="53"/>
-      <c r="N48" s="108" t="s">
+      <c r="N48" s="107" t="s">
         <v>230</v>
       </c>
-      <c r="O48" s="108"/>
+      <c r="O48" s="107"/>
       <c r="P48" s="38" t="s">
         <v>231</v>
       </c>
       <c r="Q48" s="38"/>
       <c r="R48" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S48" s="59"/>
       <c r="T48" s="49" t="s">
@@ -4777,18 +4771,18 @@
       </c>
     </row>
     <row r="51" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B51" s="119" t="s">
+      <c r="B51" s="118" t="s">
         <v>232</v>
       </c>
-      <c r="C51" s="119"/>
+      <c r="C51" s="118"/>
       <c r="D51" s="38" t="s">
         <v>233</v>
       </c>
       <c r="E51" s="38"/>
-      <c r="F51" s="119" t="s">
+      <c r="F51" s="118" t="s">
         <v>234</v>
       </c>
-      <c r="G51" s="119"/>
+      <c r="G51" s="118"/>
       <c r="H51" s="38" t="s">
         <v>235</v>
       </c>
@@ -4853,10 +4847,10 @@
         <v>247</v>
       </c>
       <c r="M52" s="38"/>
-      <c r="N52" s="108" t="s">
+      <c r="N52" s="107" t="s">
         <v>248</v>
       </c>
-      <c r="O52" s="108"/>
+      <c r="O52" s="107"/>
       <c r="P52" s="38" t="s">
         <v>249</v>
       </c>
@@ -4869,10 +4863,10 @@
         <v>254</v>
       </c>
       <c r="U52" s="38"/>
-      <c r="V52" s="106" t="s">
+      <c r="V52" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W52" s="106"/>
+      <c r="W52" s="105"/>
       <c r="AA52" s="8"/>
       <c r="AB52" s="8"/>
       <c r="AC52" s="8"/>
@@ -4964,38 +4958,38 @@
     </row>
     <row r="54" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="1"/>
-      <c r="B54" s="103" t="s">
+      <c r="B54" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="103"/>
-      <c r="D54" s="103" t="s">
+      <c r="C54" s="101"/>
+      <c r="D54" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E54" s="103"/>
-      <c r="F54" s="103" t="s">
+      <c r="E54" s="101"/>
+      <c r="F54" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G54" s="103"/>
-      <c r="H54" s="108" t="s">
+      <c r="G54" s="101"/>
+      <c r="H54" s="107" t="s">
         <v>262</v>
       </c>
-      <c r="I54" s="108"/>
+      <c r="I54" s="107"/>
       <c r="J54" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K54" s="53"/>
       <c r="L54" s="53"/>
       <c r="M54" s="53"/>
-      <c r="N54" s="119" t="s">
+      <c r="N54" s="118" t="s">
         <v>263</v>
       </c>
-      <c r="O54" s="119"/>
+      <c r="O54" s="118"/>
       <c r="P54" s="38" t="s">
         <v>264</v>
       </c>
       <c r="Q54" s="38"/>
       <c r="R54" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S54" s="59"/>
       <c r="T54" s="49" t="s">
@@ -5068,10 +5062,10 @@
       </c>
     </row>
     <row r="57" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="119" t="s">
+      <c r="B57" s="118" t="s">
         <v>265</v>
       </c>
-      <c r="C57" s="119"/>
+      <c r="C57" s="118"/>
       <c r="D57" s="38" t="s">
         <v>266</v>
       </c>
@@ -5160,10 +5154,10 @@
         <v>284</v>
       </c>
       <c r="U58" s="38"/>
-      <c r="V58" s="106" t="s">
+      <c r="V58" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="W58" s="106"/>
+      <c r="W58" s="105"/>
       <c r="AA58" s="8"/>
       <c r="AB58" s="8"/>
       <c r="AC58" s="8"/>
@@ -5251,32 +5245,32 @@
     </row>
     <row r="60" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="1"/>
-      <c r="B60" s="103" t="s">
+      <c r="B60" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C60" s="103"/>
-      <c r="D60" s="103" t="s">
+      <c r="C60" s="101"/>
+      <c r="D60" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E60" s="103"/>
-      <c r="F60" s="103" t="s">
+      <c r="E60" s="101"/>
+      <c r="F60" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G60" s="103"/>
-      <c r="H60" s="108"/>
-      <c r="I60" s="108"/>
+      <c r="G60" s="101"/>
+      <c r="H60" s="107"/>
+      <c r="I60" s="107"/>
       <c r="J60" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K60" s="53"/>
       <c r="L60" s="53"/>
       <c r="M60" s="53"/>
-      <c r="N60" s="119"/>
-      <c r="O60" s="119"/>
+      <c r="N60" s="118"/>
+      <c r="O60" s="118"/>
       <c r="P60" s="38"/>
       <c r="Q60" s="38"/>
       <c r="R60" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S60" s="59"/>
       <c r="T60" s="49" t="s">
@@ -5352,46 +5346,46 @@
       </c>
     </row>
     <row r="63" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C63" s="77" t="s">
+      <c r="C63" s="75" t="s">
         <v>87</v>
       </c>
-      <c r="D63" s="77"/>
-      <c r="E63" s="77" t="s">
+      <c r="D63" s="75"/>
+      <c r="E63" s="75" t="s">
         <v>88</v>
       </c>
-      <c r="F63" s="77"/>
-      <c r="G63" s="77" t="s">
+      <c r="F63" s="75"/>
+      <c r="G63" s="75" t="s">
         <v>89</v>
       </c>
-      <c r="H63" s="77"/>
-      <c r="I63" s="77" t="s">
+      <c r="H63" s="75"/>
+      <c r="I63" s="75" t="s">
         <v>90</v>
       </c>
-      <c r="J63" s="77"/>
-      <c r="K63" s="77" t="s">
+      <c r="J63" s="75"/>
+      <c r="K63" s="75" t="s">
         <v>91</v>
       </c>
-      <c r="L63" s="77"/>
-      <c r="M63" s="77" t="s">
+      <c r="L63" s="75"/>
+      <c r="M63" s="75" t="s">
         <v>92</v>
       </c>
-      <c r="N63" s="77"/>
-      <c r="O63" s="77" t="s">
+      <c r="N63" s="75"/>
+      <c r="O63" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="P63" s="77"/>
-      <c r="Q63" s="77" t="s">
+      <c r="P63" s="75"/>
+      <c r="Q63" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="R63" s="77"/>
-      <c r="S63" s="77" t="s">
+      <c r="R63" s="75"/>
+      <c r="S63" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="T63" s="77"/>
-      <c r="U63" s="77" t="s">
+      <c r="T63" s="75"/>
+      <c r="U63" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="V63" s="77"/>
+      <c r="V63" s="75"/>
       <c r="W63" s="5"/>
       <c r="X63" s="5"/>
       <c r="Y63" s="5"/>
@@ -5400,14 +5394,14 @@
     </row>
     <row r="64" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="1"/>
-      <c r="B64" s="79" t="s">
+      <c r="B64" s="77" t="s">
         <v>85</v>
       </c>
-      <c r="C64" s="80"/>
-      <c r="D64" s="79" t="s">
+      <c r="C64" s="78"/>
+      <c r="D64" s="77" t="s">
         <v>113</v>
       </c>
-      <c r="E64" s="80"/>
+      <c r="E64" s="78"/>
       <c r="F64" s="69" t="s">
         <v>108</v>
       </c>
@@ -5416,30 +5410,30 @@
         <v>109</v>
       </c>
       <c r="I64" s="69"/>
-      <c r="J64" s="81" t="s">
+      <c r="J64" s="79" t="s">
         <v>104</v>
       </c>
-      <c r="K64" s="82"/>
-      <c r="L64" s="81" t="s">
+      <c r="K64" s="80"/>
+      <c r="L64" s="79" t="s">
         <v>100</v>
       </c>
-      <c r="M64" s="82"/>
-      <c r="N64" s="81" t="s">
+      <c r="M64" s="80"/>
+      <c r="N64" s="79" t="s">
         <v>105</v>
       </c>
-      <c r="O64" s="82"/>
-      <c r="P64" s="79" t="s">
+      <c r="O64" s="80"/>
+      <c r="P64" s="77" t="s">
         <v>107</v>
       </c>
-      <c r="Q64" s="80"/>
-      <c r="R64" s="79" t="s">
+      <c r="Q64" s="78"/>
+      <c r="R64" s="77" t="s">
         <v>97</v>
       </c>
-      <c r="S64" s="80"/>
-      <c r="T64" s="79" t="s">
+      <c r="S64" s="78"/>
+      <c r="T64" s="77" t="s">
         <v>98</v>
       </c>
-      <c r="U64" s="80"/>
+      <c r="U64" s="78"/>
       <c r="V64" s="70" t="s">
         <v>37</v>
       </c>
@@ -5451,34 +5445,34 @@
         <v>27</v>
       </c>
       <c r="C65" s="38"/>
-      <c r="D65" s="81" t="s">
+      <c r="D65" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="E65" s="82"/>
-      <c r="F65" s="81" t="s">
+      <c r="E65" s="80"/>
+      <c r="F65" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="G65" s="82"/>
-      <c r="H65" s="81" t="s">
+      <c r="G65" s="80"/>
+      <c r="H65" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="I65" s="82"/>
-      <c r="J65" s="79" t="s">
+      <c r="I65" s="80"/>
+      <c r="J65" s="77" t="s">
         <v>102</v>
       </c>
-      <c r="K65" s="80"/>
-      <c r="L65" s="79" t="s">
+      <c r="K65" s="78"/>
+      <c r="L65" s="77" t="s">
         <v>101</v>
       </c>
-      <c r="M65" s="80"/>
-      <c r="N65" s="79" t="s">
+      <c r="M65" s="78"/>
+      <c r="N65" s="77" t="s">
         <v>103</v>
       </c>
-      <c r="O65" s="80"/>
-      <c r="P65" s="81" t="s">
+      <c r="O65" s="78"/>
+      <c r="P65" s="79" t="s">
         <v>106</v>
       </c>
-      <c r="Q65" s="82"/>
+      <c r="Q65" s="80"/>
       <c r="R65" s="56" t="s">
         <v>99</v>
       </c>
@@ -5487,41 +5481,41 @@
         <v>30</v>
       </c>
       <c r="U65" s="56"/>
-      <c r="V65" s="78" t="s">
+      <c r="V65" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="W65" s="78"/>
+      <c r="W65" s="76"/>
     </row>
     <row r="66" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="1"/>
-      <c r="B66" s="103" t="s">
+      <c r="B66" s="101" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="103"/>
-      <c r="D66" s="103" t="s">
+      <c r="C66" s="101"/>
+      <c r="D66" s="101" t="s">
         <v>35</v>
       </c>
-      <c r="E66" s="103"/>
-      <c r="F66" s="103" t="s">
+      <c r="E66" s="101"/>
+      <c r="F66" s="101" t="s">
         <v>34</v>
       </c>
-      <c r="G66" s="103"/>
-      <c r="H66" s="81"/>
-      <c r="I66" s="82"/>
+      <c r="G66" s="101"/>
+      <c r="H66" s="79"/>
+      <c r="I66" s="80"/>
       <c r="J66" s="51" t="s">
         <v>26</v>
       </c>
       <c r="K66" s="53"/>
       <c r="L66" s="53"/>
       <c r="M66" s="52"/>
-      <c r="N66" s="79"/>
-      <c r="O66" s="80"/>
-      <c r="P66" s="79" t="s">
+      <c r="N66" s="77"/>
+      <c r="O66" s="78"/>
+      <c r="P66" s="77" t="s">
         <v>112</v>
       </c>
-      <c r="Q66" s="80"/>
+      <c r="Q66" s="78"/>
       <c r="R66" s="59" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="S66" s="59"/>
       <c r="T66" s="49" t="s">
@@ -5545,32 +5539,32 @@
         <v>73</v>
       </c>
       <c r="C69" s="25"/>
-      <c r="D69" s="132" t="s">
+      <c r="D69" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="E69" s="133"/>
-      <c r="F69" s="133"/>
-      <c r="G69" s="133"/>
-      <c r="H69" s="134"/>
-      <c r="I69" s="132" t="s">
+      <c r="E69" s="132"/>
+      <c r="F69" s="132"/>
+      <c r="G69" s="132"/>
+      <c r="H69" s="133"/>
+      <c r="I69" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="J69" s="133"/>
-      <c r="K69" s="133"/>
-      <c r="L69" s="133"/>
-      <c r="M69" s="132" t="s">
+      <c r="J69" s="132"/>
+      <c r="K69" s="132"/>
+      <c r="L69" s="132"/>
+      <c r="M69" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="N69" s="133"/>
-      <c r="O69" s="133"/>
-      <c r="P69" s="133"/>
-      <c r="Q69" s="132" t="s">
+      <c r="N69" s="132"/>
+      <c r="O69" s="132"/>
+      <c r="P69" s="132"/>
+      <c r="Q69" s="131" t="s">
         <v>120</v>
       </c>
-      <c r="R69" s="133"/>
-      <c r="S69" s="133"/>
-      <c r="T69" s="133"/>
-      <c r="U69" s="134"/>
+      <c r="R69" s="132"/>
+      <c r="S69" s="132"/>
+      <c r="T69" s="132"/>
+      <c r="U69" s="133"/>
       <c r="V69" s="24" t="s">
         <v>74</v>
       </c>
@@ -5598,21 +5592,19 @@
     </row>
     <row r="70" spans="1:49" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="1"/>
-      <c r="B70" s="104" t="s">
+      <c r="B70" s="102" t="s">
         <v>119</v>
       </c>
-      <c r="C70" s="105"/>
-      <c r="D70" s="131" t="s">
+      <c r="C70" s="103"/>
+      <c r="D70" s="130" t="s">
         <v>201</v>
       </c>
-      <c r="E70" s="105"/>
-      <c r="F70" s="71" t="s">
-        <v>118</v>
-      </c>
-      <c r="G70" s="72"/>
-      <c r="H70" s="33" t="s">
-        <v>332</v>
-      </c>
+      <c r="E70" s="103"/>
+      <c r="F70" s="33" t="s">
+        <v>331</v>
+      </c>
+      <c r="G70" s="34"/>
+      <c r="H70" s="34"/>
       <c r="I70" s="34"/>
       <c r="J70" s="34"/>
       <c r="K70" s="34"/>
@@ -5622,18 +5614,16 @@
       <c r="O70" s="34"/>
       <c r="P70" s="34"/>
       <c r="Q70" s="34"/>
-      <c r="R70" s="73" t="s">
+      <c r="R70" s="34"/>
+      <c r="S70" s="104"/>
+      <c r="T70" s="71" t="s">
+        <v>118</v>
+      </c>
+      <c r="U70" s="72"/>
+      <c r="V70" s="128" t="s">
         <v>328</v>
       </c>
-      <c r="S70" s="74"/>
-      <c r="T70" s="129" t="s">
-        <v>329</v>
-      </c>
-      <c r="U70" s="130"/>
-      <c r="V70" s="73" t="s">
-        <v>320</v>
-      </c>
-      <c r="W70" s="74"/>
+      <c r="W70" s="129"/>
       <c r="Z70" s="5"/>
       <c r="AA70" s="8"/>
       <c r="AB70" s="8"/>
@@ -5657,7 +5647,7 @@
     </row>
     <row r="72" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B72" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="73" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -5688,13 +5678,13 @@
       <c r="P73" s="68" t="s">
         <v>306</v>
       </c>
-      <c r="Q73" s="84"/>
-      <c r="R73" s="85"/>
-      <c r="S73" s="120" t="s">
+      <c r="Q73" s="82"/>
+      <c r="R73" s="83"/>
+      <c r="S73" s="119" t="s">
         <v>307</v>
       </c>
-      <c r="T73" s="121"/>
-      <c r="U73" s="122"/>
+      <c r="T73" s="120"/>
+      <c r="U73" s="121"/>
     </row>
     <row r="74" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B74" s="60" t="s">
@@ -5721,12 +5711,12 @@
         <v>5</v>
       </c>
       <c r="N74" s="61"/>
-      <c r="P74" s="86"/>
-      <c r="Q74" s="87"/>
-      <c r="R74" s="88"/>
-      <c r="S74" s="123"/>
-      <c r="T74" s="124"/>
-      <c r="U74" s="125"/>
+      <c r="P74" s="84"/>
+      <c r="Q74" s="85"/>
+      <c r="R74" s="86"/>
+      <c r="S74" s="122"/>
+      <c r="T74" s="123"/>
+      <c r="U74" s="124"/>
     </row>
     <row r="75" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B75" s="60" t="s">
@@ -5740,7 +5730,7 @@
       <c r="F75" s="68" t="s">
         <v>304</v>
       </c>
-      <c r="G75" s="85"/>
+      <c r="G75" s="83"/>
       <c r="I75" s="68" t="s">
         <v>303</v>
       </c>
@@ -5756,11 +5746,11 @@
       <c r="P75" s="68" t="s">
         <v>310</v>
       </c>
-      <c r="Q75" s="84"/>
-      <c r="R75" s="84"/>
-      <c r="S75" s="84"/>
-      <c r="T75" s="84"/>
-      <c r="U75" s="85"/>
+      <c r="Q75" s="82"/>
+      <c r="R75" s="82"/>
+      <c r="S75" s="82"/>
+      <c r="T75" s="82"/>
+      <c r="U75" s="83"/>
     </row>
     <row r="76" spans="1:49" ht="10.199999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B76" s="12"/>
@@ -5775,12 +5765,12 @@
       <c r="L76" s="15"/>
       <c r="M76" s="15"/>
       <c r="N76" s="16"/>
-      <c r="P76" s="126"/>
-      <c r="Q76" s="127"/>
-      <c r="R76" s="127"/>
-      <c r="S76" s="127"/>
-      <c r="T76" s="127"/>
-      <c r="U76" s="128"/>
+      <c r="P76" s="125"/>
+      <c r="Q76" s="126"/>
+      <c r="R76" s="126"/>
+      <c r="S76" s="126"/>
+      <c r="T76" s="126"/>
+      <c r="U76" s="127"/>
       <c r="W76" s="22"/>
       <c r="X76" s="22"/>
       <c r="Y76" s="22"/>
@@ -5792,33 +5782,33 @@
       <c r="B77" s="60" t="s">
         <v>305</v>
       </c>
-      <c r="C77" s="83"/>
-      <c r="D77" s="83"/>
-      <c r="E77" s="83"/>
-      <c r="F77" s="83"/>
+      <c r="C77" s="81"/>
+      <c r="D77" s="81"/>
+      <c r="E77" s="81"/>
+      <c r="F77" s="81"/>
       <c r="G77" s="61"/>
       <c r="H77" s="11"/>
       <c r="I77" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="J77" s="83"/>
+      <c r="J77" s="81"/>
       <c r="K77" s="61"/>
       <c r="L77" s="60" t="s">
         <v>309</v>
       </c>
-      <c r="M77" s="83"/>
+      <c r="M77" s="81"/>
       <c r="N77" s="61"/>
-      <c r="P77" s="86"/>
-      <c r="Q77" s="87"/>
-      <c r="R77" s="87"/>
-      <c r="S77" s="87"/>
-      <c r="T77" s="87"/>
-      <c r="U77" s="88"/>
+      <c r="P77" s="84"/>
+      <c r="Q77" s="85"/>
+      <c r="R77" s="85"/>
+      <c r="S77" s="85"/>
+      <c r="T77" s="85"/>
+      <c r="U77" s="86"/>
       <c r="V77" s="11"/>
     </row>
     <row r="79" spans="1:49" x14ac:dyDescent="0.3">
       <c r="B79" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="80" spans="1:49" ht="30" customHeight="1" x14ac:dyDescent="0.3">
@@ -5849,13 +5839,13 @@
       <c r="P80" s="68" t="s">
         <v>306</v>
       </c>
-      <c r="Q80" s="84"/>
-      <c r="R80" s="85"/>
-      <c r="S80" s="120" t="s">
+      <c r="Q80" s="82"/>
+      <c r="R80" s="83"/>
+      <c r="S80" s="119" t="s">
         <v>307</v>
       </c>
-      <c r="T80" s="121"/>
-      <c r="U80" s="122"/>
+      <c r="T80" s="120"/>
+      <c r="U80" s="121"/>
     </row>
     <row r="81" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B81" s="60" t="s">
@@ -5882,26 +5872,26 @@
         <v>5</v>
       </c>
       <c r="N81" s="61"/>
-      <c r="P81" s="86"/>
-      <c r="Q81" s="87"/>
-      <c r="R81" s="88"/>
-      <c r="S81" s="123"/>
-      <c r="T81" s="124"/>
-      <c r="U81" s="125"/>
+      <c r="P81" s="84"/>
+      <c r="Q81" s="85"/>
+      <c r="R81" s="86"/>
+      <c r="S81" s="122"/>
+      <c r="T81" s="123"/>
+      <c r="U81" s="124"/>
     </row>
     <row r="82" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B82" s="68" t="s">
         <v>303</v>
       </c>
-      <c r="C82" s="85"/>
+      <c r="C82" s="83"/>
       <c r="D82" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="E82" s="85"/>
+      <c r="E82" s="83"/>
       <c r="F82" s="68" t="s">
         <v>304</v>
       </c>
-      <c r="G82" s="85"/>
+      <c r="G82" s="83"/>
       <c r="I82" s="60" t="s">
         <v>303</v>
       </c>
@@ -5917,11 +5907,11 @@
       <c r="P82" s="68" t="s">
         <v>310</v>
       </c>
-      <c r="Q82" s="84"/>
-      <c r="R82" s="84"/>
-      <c r="S82" s="84"/>
-      <c r="T82" s="84"/>
-      <c r="U82" s="85"/>
+      <c r="Q82" s="82"/>
+      <c r="R82" s="82"/>
+      <c r="S82" s="82"/>
+      <c r="T82" s="82"/>
+      <c r="U82" s="83"/>
       <c r="V82" s="23"/>
       <c r="W82" s="23"/>
       <c r="X82" s="23"/>
@@ -5943,12 +5933,12 @@
       <c r="L83" s="17"/>
       <c r="M83" s="17"/>
       <c r="N83" s="18"/>
-      <c r="P83" s="126"/>
-      <c r="Q83" s="127"/>
-      <c r="R83" s="127"/>
-      <c r="S83" s="127"/>
-      <c r="T83" s="127"/>
-      <c r="U83" s="128"/>
+      <c r="P83" s="125"/>
+      <c r="Q83" s="126"/>
+      <c r="R83" s="126"/>
+      <c r="S83" s="126"/>
+      <c r="T83" s="126"/>
+      <c r="U83" s="127"/>
       <c r="W83" s="22"/>
       <c r="X83" s="22"/>
       <c r="Y83" s="22"/>
@@ -5960,35 +5950,35 @@
       <c r="B84" s="60" t="s">
         <v>305</v>
       </c>
-      <c r="C84" s="83"/>
-      <c r="D84" s="83"/>
-      <c r="E84" s="83"/>
-      <c r="F84" s="83"/>
+      <c r="C84" s="81"/>
+      <c r="D84" s="81"/>
+      <c r="E84" s="81"/>
+      <c r="F84" s="81"/>
       <c r="G84" s="61"/>
       <c r="H84" s="11"/>
       <c r="I84" s="60" t="s">
         <v>308</v>
       </c>
-      <c r="J84" s="83"/>
+      <c r="J84" s="81"/>
       <c r="K84" s="61"/>
       <c r="L84" s="60" t="s">
         <v>309</v>
       </c>
-      <c r="M84" s="83"/>
+      <c r="M84" s="81"/>
       <c r="N84" s="61"/>
-      <c r="P84" s="86"/>
-      <c r="Q84" s="87"/>
-      <c r="R84" s="87"/>
-      <c r="S84" s="87"/>
-      <c r="T84" s="87"/>
-      <c r="U84" s="88"/>
+      <c r="P84" s="84"/>
+      <c r="Q84" s="85"/>
+      <c r="R84" s="85"/>
+      <c r="S84" s="85"/>
+      <c r="T84" s="85"/>
+      <c r="U84" s="86"/>
       <c r="V84" s="11"/>
-      <c r="W84" s="127"/>
-      <c r="X84" s="127"/>
-      <c r="Y84" s="127"/>
-      <c r="Z84" s="127"/>
-      <c r="AA84" s="127"/>
-      <c r="AB84" s="127"/>
+      <c r="W84" s="126"/>
+      <c r="X84" s="126"/>
+      <c r="Y84" s="126"/>
+      <c r="Z84" s="126"/>
+      <c r="AA84" s="126"/>
+      <c r="AB84" s="126"/>
     </row>
     <row r="86" spans="2:32" x14ac:dyDescent="0.3">
       <c r="B86" s="10" t="s">
@@ -5999,21 +5989,21 @@
       <c r="B87" s="68" t="s">
         <v>314</v>
       </c>
-      <c r="C87" s="84"/>
-      <c r="D87" s="84"/>
-      <c r="E87" s="85"/>
-      <c r="F87" s="95" t="s">
-        <v>323</v>
-      </c>
-      <c r="G87" s="96"/>
-      <c r="H87" s="96"/>
-      <c r="I87" s="97"/>
+      <c r="C87" s="82"/>
+      <c r="D87" s="82"/>
+      <c r="E87" s="83"/>
+      <c r="F87" s="93" t="s">
+        <v>322</v>
+      </c>
+      <c r="G87" s="94"/>
+      <c r="H87" s="94"/>
+      <c r="I87" s="95"/>
       <c r="J87" s="68" t="s">
         <v>316</v>
       </c>
-      <c r="K87" s="84"/>
-      <c r="L87" s="84"/>
-      <c r="M87" s="85"/>
+      <c r="K87" s="82"/>
+      <c r="L87" s="82"/>
+      <c r="M87" s="83"/>
       <c r="O87" s="60" t="s">
         <v>298</v>
       </c>
@@ -6027,12 +6017,12 @@
       </c>
       <c r="T87" s="61"/>
       <c r="U87" s="11"/>
-      <c r="V87" s="89" t="s">
+      <c r="V87" s="87" t="s">
         <v>318</v>
       </c>
-      <c r="W87" s="90"/>
-      <c r="X87" s="90"/>
-      <c r="Y87" s="91"/>
+      <c r="W87" s="88"/>
+      <c r="X87" s="88"/>
+      <c r="Y87" s="89"/>
       <c r="Z87" s="60" t="s">
         <v>27</v>
       </c>
@@ -6044,18 +6034,18 @@
       <c r="AD87" s="11"/>
     </row>
     <row r="88" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B88" s="86"/>
-      <c r="C88" s="87"/>
-      <c r="D88" s="87"/>
-      <c r="E88" s="88"/>
-      <c r="F88" s="98"/>
-      <c r="G88" s="99"/>
-      <c r="H88" s="99"/>
-      <c r="I88" s="100"/>
-      <c r="J88" s="86"/>
-      <c r="K88" s="87"/>
-      <c r="L88" s="87"/>
-      <c r="M88" s="88"/>
+      <c r="B88" s="84"/>
+      <c r="C88" s="85"/>
+      <c r="D88" s="85"/>
+      <c r="E88" s="86"/>
+      <c r="F88" s="96"/>
+      <c r="G88" s="97"/>
+      <c r="H88" s="97"/>
+      <c r="I88" s="98"/>
+      <c r="J88" s="84"/>
+      <c r="K88" s="85"/>
+      <c r="L88" s="85"/>
+      <c r="M88" s="86"/>
       <c r="O88" s="60" t="s">
         <v>18</v>
       </c>
@@ -6069,10 +6059,10 @@
       </c>
       <c r="T88" s="61"/>
       <c r="U88" s="11"/>
-      <c r="V88" s="92"/>
-      <c r="W88" s="93"/>
-      <c r="X88" s="93"/>
-      <c r="Y88" s="94"/>
+      <c r="V88" s="90"/>
+      <c r="W88" s="91"/>
+      <c r="X88" s="91"/>
+      <c r="Y88" s="92"/>
       <c r="Z88" s="60" t="s">
         <v>32</v>
       </c>
@@ -6084,24 +6074,24 @@
       <c r="AD88" s="11"/>
     </row>
     <row r="89" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B89" s="89" t="s">
+      <c r="B89" s="87" t="s">
         <v>315</v>
       </c>
-      <c r="C89" s="90"/>
-      <c r="D89" s="90"/>
-      <c r="E89" s="91"/>
+      <c r="C89" s="88"/>
+      <c r="D89" s="88"/>
+      <c r="E89" s="89"/>
       <c r="F89" s="68" t="s">
         <v>313</v>
       </c>
-      <c r="G89" s="84"/>
-      <c r="H89" s="84"/>
-      <c r="I89" s="85"/>
-      <c r="J89" s="95" t="s">
+      <c r="G89" s="82"/>
+      <c r="H89" s="82"/>
+      <c r="I89" s="83"/>
+      <c r="J89" s="93" t="s">
         <v>319</v>
       </c>
-      <c r="K89" s="96"/>
-      <c r="L89" s="96"/>
-      <c r="M89" s="97"/>
+      <c r="K89" s="94"/>
+      <c r="L89" s="94"/>
+      <c r="M89" s="95"/>
       <c r="O89" s="60" t="s">
         <v>303</v>
       </c>
@@ -6118,47 +6108,47 @@
       <c r="V89" s="68" t="s">
         <v>297</v>
       </c>
-      <c r="W89" s="84"/>
-      <c r="X89" s="84"/>
-      <c r="Y89" s="84"/>
-      <c r="Z89" s="84"/>
-      <c r="AA89" s="84"/>
-      <c r="AB89" s="84"/>
-      <c r="AC89" s="85"/>
+      <c r="W89" s="82"/>
+      <c r="X89" s="82"/>
+      <c r="Y89" s="82"/>
+      <c r="Z89" s="82"/>
+      <c r="AA89" s="82"/>
+      <c r="AB89" s="82"/>
+      <c r="AC89" s="83"/>
       <c r="AD89" s="11"/>
       <c r="AE89" s="11"/>
       <c r="AF89" s="11"/>
     </row>
     <row r="90" spans="2:32" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B90" s="92"/>
-      <c r="C90" s="93"/>
-      <c r="D90" s="93"/>
-      <c r="E90" s="94"/>
-      <c r="F90" s="86"/>
-      <c r="G90" s="87"/>
-      <c r="H90" s="87"/>
-      <c r="I90" s="88"/>
-      <c r="J90" s="98"/>
-      <c r="K90" s="99"/>
-      <c r="L90" s="99"/>
-      <c r="M90" s="100"/>
+      <c r="B90" s="90"/>
+      <c r="C90" s="91"/>
+      <c r="D90" s="91"/>
+      <c r="E90" s="92"/>
+      <c r="F90" s="84"/>
+      <c r="G90" s="85"/>
+      <c r="H90" s="85"/>
+      <c r="I90" s="86"/>
+      <c r="J90" s="96"/>
+      <c r="K90" s="97"/>
+      <c r="L90" s="97"/>
+      <c r="M90" s="98"/>
       <c r="O90" s="60" t="s">
         <v>317</v>
       </c>
-      <c r="P90" s="83"/>
-      <c r="Q90" s="83"/>
-      <c r="R90" s="83"/>
-      <c r="S90" s="83"/>
+      <c r="P90" s="81"/>
+      <c r="Q90" s="81"/>
+      <c r="R90" s="81"/>
+      <c r="S90" s="81"/>
       <c r="T90" s="61"/>
       <c r="U90" s="11"/>
-      <c r="V90" s="86"/>
-      <c r="W90" s="87"/>
-      <c r="X90" s="87"/>
-      <c r="Y90" s="87"/>
-      <c r="Z90" s="87"/>
-      <c r="AA90" s="87"/>
-      <c r="AB90" s="87"/>
-      <c r="AC90" s="88"/>
+      <c r="V90" s="84"/>
+      <c r="W90" s="85"/>
+      <c r="X90" s="85"/>
+      <c r="Y90" s="85"/>
+      <c r="Z90" s="85"/>
+      <c r="AA90" s="85"/>
+      <c r="AB90" s="85"/>
+      <c r="AC90" s="86"/>
       <c r="AD90" s="11"/>
       <c r="AE90" s="11"/>
       <c r="AF90" s="11"/>
@@ -6275,9 +6265,10 @@
       <c r="B164" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="520">
+  <mergeCells count="518">
     <mergeCell ref="D69:H69"/>
     <mergeCell ref="Q69:U69"/>
+    <mergeCell ref="F70:S70"/>
     <mergeCell ref="I69:L69"/>
     <mergeCell ref="M69:P69"/>
     <mergeCell ref="Z88:AA88"/>
@@ -6671,9 +6662,6 @@
     <mergeCell ref="T70:U70"/>
     <mergeCell ref="V70:W70"/>
     <mergeCell ref="B69:C69"/>
-    <mergeCell ref="F70:G70"/>
-    <mergeCell ref="H70:Q70"/>
-    <mergeCell ref="R70:S70"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>

</xml_diff>